<commit_message>
replace postgres table if exists, automate excel columns
</commit_message>
<xml_diff>
--- a/pure_crypto_companies.xlsx
+++ b/pure_crypto_companies.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholaslor/Desktop/MENG/bill-tracker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholaslor/Desktop/MENG/crypto-lobbying-tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624E61E9-484C-F445-908A-CDF192581D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3ABFCA-02AC-124B-9F17-0664D54E02B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{0B7C7B67-ED92-B34A-93F9-EF38BA225A91}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{0B7C7B67-ED92-B34A-93F9-EF38BA225A91}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="113">
   <si>
     <t>Row Labels</t>
   </si>
@@ -371,7 +371,10 @@
     <t>Merged Company Name</t>
   </si>
   <si>
-    <t>Original Client Name</t>
+    <t>client.name</t>
+  </si>
+  <si>
+    <t>merged_client.name</t>
   </si>
 </sst>
 </file>
@@ -381,9 +384,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -404,7 +415,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -412,11 +423,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -432,6 +458,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -781,7 +810,7 @@
   <dimension ref="A1:B102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -791,11 +820,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>111</v>
       </c>
       <c r="B1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>